<commit_message>
checking with origin -u remote
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ATUL KUMAR\OneDrive\Desktop\calculater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E42F9A5-A44D-4E85-863C-6B4E5D14EAE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7975ED28-8170-4870-924C-49CE6B4D4BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4716" yWindow="2052" windowWidth="17280" windowHeight="8964" xr2:uid="{A6574F2C-8269-4FC8-BA92-01B68C7507D3}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">hi </t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>dfsf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">atul </t>
+  </si>
+  <si>
+    <t xml:space="preserve">aj </t>
   </si>
 </sst>
 </file>
@@ -401,35 +407,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03398DF8-84DF-4EA4-ACA9-0BFC4951EBB6}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>5</v>
       </c>

</xml_diff>